<commit_message>
Oct 21 Standup Meeting
</commit_message>
<xml_diff>
--- a/docs/planning/burndown-charts.xlsx
+++ b/docs/planning/burndown-charts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dyl2e\USU\SoftwareEngineering\dans-frappy-shop\docs\scrum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\School\Fall 2022\CS 3450\Main Project\frappy\docs\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D3E202-458E-45DD-ACD9-E01A0F210C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDD14CA-4114-4309-8CA8-DABCB7E8C57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="510" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Milestone 1" sheetId="2" r:id="rId1"/>
@@ -27,12 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -227,17 +224,17 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3637,13 +3634,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -3787,28 +3784,28 @@
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>33</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8784,23 +8781,22 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" customWidth="1"/>
-    <col min="8" max="9" width="7.33203125" customWidth="1"/>
-    <col min="10" max="12" width="7.21875" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="12" width="7.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -8841,7 +8837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -8883,7 +8879,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -8925,7 +8921,7 @@
         <v>-0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -8967,7 +8963,7 @@
         <v>-0.75</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -9009,7 +9005,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -9047,7 +9043,7 @@
         <v>44820</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>3</v>
       </c>
@@ -9093,7 +9089,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>6</v>
       </c>
@@ -9139,7 +9135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>1</v>
       </c>
@@ -9188,7 +9184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>4</v>
       </c>
@@ -9252,23 +9248,22 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" customWidth="1"/>
-    <col min="8" max="9" width="7.33203125" customWidth="1"/>
-    <col min="10" max="13" width="7.21875" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="13" width="7.28515625" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -9312,7 +9307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -9355,7 +9350,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -9398,7 +9393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -9441,7 +9436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -9484,7 +9479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -9523,7 +9518,7 @@
       </c>
       <c r="M8" s="16"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>3</v>
       </c>
@@ -9570,7 +9565,7 @@
       </c>
       <c r="M9" s="5"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>6</v>
       </c>
@@ -9617,7 +9612,7 @@
       </c>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>1</v>
       </c>
@@ -9666,7 +9661,7 @@
       </c>
       <c r="M11" s="5"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>4</v>
       </c>
@@ -9730,23 +9725,22 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" customWidth="1"/>
-    <col min="8" max="9" width="7.33203125" customWidth="1"/>
-    <col min="10" max="12" width="7.21875" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="12" width="7.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -9787,7 +9781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -9830,7 +9824,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -9873,7 +9867,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -9916,7 +9910,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -9959,7 +9953,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -10007,7 +10001,7 @@
         <v>44848</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>3</v>
       </c>
@@ -10053,7 +10047,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>6</v>
       </c>
@@ -10099,7 +10093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>1</v>
       </c>
@@ -10148,7 +10142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>4</v>
       </c>
@@ -10197,7 +10191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -10216,27 +10210,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DEB9ECB-E51C-4BE8-90E7-4F5475BC515A}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="102" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" customWidth="1"/>
-    <col min="8" max="9" width="7.33203125" customWidth="1"/>
-    <col min="10" max="12" width="7.21875" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="12" width="7.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -10277,7 +10270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -10298,7 +10291,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H2" s="5">
         <v>0</v>
@@ -10317,10 +10310,10 @@
       </c>
       <c r="M2" s="10">
         <f>B2-(SUM(C2:L2))</f>
-        <v>8.25</v>
+        <v>6.25</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -10363,7 +10356,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -10406,7 +10399,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -10421,7 +10414,7 @@
         <v>0.25</v>
       </c>
       <c r="E5" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F5" s="7">
         <v>0</v>
@@ -10446,10 +10439,10 @@
       </c>
       <c r="M5" s="11">
         <f>B5-(SUM(C5:L5))</f>
-        <v>8.25</v>
+        <v>4.25</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -10497,7 +10490,7 @@
         <v>44862</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>3</v>
       </c>
@@ -10543,7 +10536,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>6</v>
       </c>
@@ -10558,7 +10551,7 @@
       </c>
       <c r="E10" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="2"/>
@@ -10566,7 +10559,7 @@
       </c>
       <c r="G10" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10" s="7">
         <f t="shared" si="2"/>
@@ -10589,7 +10582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>1</v>
       </c>
@@ -10607,38 +10600,38 @@
       </c>
       <c r="E11" s="5">
         <f t="shared" si="3"/>
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="3"/>
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="3"/>
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="3"/>
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="3"/>
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="J11" s="5">
         <f>I11-J10</f>
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="K11" s="5">
         <f>J11-K10</f>
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="L11" s="5">
         <f>K11-L10</f>
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>4</v>
       </c>
@@ -10687,7 +10680,7 @@
         <v>6.2172489379008766E-15</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -10710,23 +10703,22 @@
       <selection activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" customWidth="1"/>
-    <col min="8" max="9" width="7.33203125" customWidth="1"/>
-    <col min="10" max="15" width="7.21875" customWidth="1"/>
-    <col min="16" max="16" width="10.109375" customWidth="1"/>
-    <col min="17" max="17" width="11.44140625" customWidth="1"/>
-    <col min="18" max="18" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="15" width="7.28515625" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -10776,7 +10768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -10828,7 +10820,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -10880,7 +10872,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -10932,7 +10924,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -10984,7 +10976,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -11044,7 +11036,7 @@
         <v>44881</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>3</v>
       </c>
@@ -11102,7 +11094,7 @@
         <v>2.9230769230769229</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>6</v>
       </c>
@@ -11160,7 +11152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>1</v>
       </c>
@@ -11221,7 +11213,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>4</v>
       </c>
@@ -11282,7 +11274,7 @@
         <v>8.7692307692307736</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Updated Last Week of Standups
</commit_message>
<xml_diff>
--- a/docs/planning/burndown-charts.xlsx
+++ b/docs/planning/burndown-charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\School\Fall 2022\CS 3450\Main Project\frappy\docs\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDA8EC9-1AB6-4E66-85EB-7399BE92610A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D29C96-407E-42E0-9DF2-3DAD3BCB9EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3721,7 +3721,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3730,7 +3730,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -3919,37 +3919,37 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>22</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>22</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>22</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10322,8 +10322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DEB9ECB-E51C-4BE8-90E7-4F5475BC515A}">
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10433,7 +10433,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="5">
         <v>0</v>
@@ -10442,7 +10442,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N2" s="5">
         <v>0</v>
@@ -10467,7 +10467,7 @@
       </c>
       <c r="U2" s="10">
         <f>B2-(SUM(C2:T2))</f>
-        <v>7.25</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -10863,7 +10863,7 @@
       </c>
       <c r="J10" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="8">
         <f t="shared" si="5"/>
@@ -10875,7 +10875,7 @@
       </c>
       <c r="M10" s="8">
         <f t="shared" ref="M10:Q10" si="6">SUM(M2:M5)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N10" s="8">
         <f t="shared" si="6"/>
@@ -10945,47 +10945,47 @@
       </c>
       <c r="J11" s="5">
         <f>I11-J10</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K11" s="5">
         <f>J11-K10</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L11" s="5">
         <f>K11-L10</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M11" s="5">
         <f t="shared" ref="M11:Q11" si="9">L11-M10</f>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="N11" s="5">
         <f t="shared" si="9"/>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="O11" s="5">
         <f t="shared" si="9"/>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="P11" s="5">
         <f t="shared" si="9"/>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="Q11" s="5">
         <f t="shared" si="9"/>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="R11" s="5">
         <f t="shared" ref="R11" si="10">Q11-R10</f>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="S11" s="5">
         <f t="shared" ref="S11" si="11">R11-S10</f>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="T11" s="5">
         <f t="shared" ref="T11" si="12">S11-T10</f>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="U11" s="5"/>
     </row>

</xml_diff>